<commit_message>
transition times refresh 2 hours before an auto transition to take into account DST
</commit_message>
<xml_diff>
--- a/hueshift2_test-cases.xlsx
+++ b/hueshift2_test-cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehol\git\github\hueshift2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27F4B152-A82F-4687-93E0-17D78DB6C045}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5CF727-4B8B-4F92-A9C3-E54BEA9DAF51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="2430" windowWidth="19395" windowHeight="9795" xr2:uid="{60309B9C-39BA-4910-A827-13BFE5EF4127}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{60309B9C-39BA-4910-A827-13BFE5EF4127}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,27 +25,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Test Case</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Completed</t>
   </si>
   <si>
-    <t>Configuration</t>
+    <t>Class/es</t>
+  </si>
+  <si>
+    <t>Behaviour</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>What happens in eg. Svalbard where there are no sunrise and sunset times? Make sure code can handle this</t>
+  </si>
+  <si>
+    <t>Changes to sunrise and sunset times, including additional hours added and removed are adhered to and transitions occur at the right time for that ACTUAL TRANSITION TIME</t>
+  </si>
+  <si>
+    <t>Transition times auto refresh two hours before a transition is supposed to happen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -60,7 +84,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -68,12 +92,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,37 +481,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C0C728-D8C6-4159-8403-2AB3F4521363}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="54" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="54" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>